<commit_message>
added some notes to the frames excel sheets
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Frames/frames for P1.xlsx
+++ b/Dataset Excel Sheets/Frames/frames for P1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaher.salman\Desktop\LINA JAN 24\Senior II\Senior-Design-Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/080c280c8b6910c1/Desktop/AUS/4. Senior Year/Spring 2024/Senior Design II/Senior-Design-Code/Dataset Excel Sheets/Frames/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_8B6C83EAB01D25C0FE15D92524B43B3D2AA0F331" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B68A9A39-F59C-420B-8612-6CA55061EBAB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7640"/>
+    <workbookView xWindow="372" yWindow="24" windowWidth="21732" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>count</t>
   </si>
@@ -50,12 +51,24 @@
   <si>
     <t>5: [159, 198]</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>No overlap between 2 &amp; 3</t>
+  </si>
+  <si>
+    <t>No overlap between 3 &amp; 4</t>
+  </si>
+  <si>
+    <t>Small overlap between 4 &amp; 5 (19 frames)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +91,14 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -239,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -274,6 +295,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,19 +600,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L459"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N459"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>2</v>
       </c>
@@ -601,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>51</v>
       </c>
@@ -627,11 +653,14 @@
       <c r="J2" s="5">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N2" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>41</v>
       </c>
@@ -659,11 +688,14 @@
       <c r="J3" s="7">
         <v>201</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N3" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>67</v>
       </c>
@@ -691,11 +723,14 @@
       <c r="J4" s="7">
         <v>180.64179100000001</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N4" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>59</v>
       </c>
@@ -723,11 +758,14 @@
       <c r="J5" s="7">
         <v>29.40954</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N5" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>61</v>
       </c>
@@ -755,11 +793,11 @@
       <c r="J6" s="7">
         <v>127</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>49</v>
       </c>
@@ -788,7 +826,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>56</v>
       </c>
@@ -817,7 +855,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>58</v>
       </c>
@@ -846,7 +884,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>54</v>
       </c>
@@ -875,7 +913,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>56</v>
       </c>
@@ -889,7 +927,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>70</v>
       </c>
@@ -903,7 +941,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>56</v>
       </c>
@@ -917,7 +955,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>57</v>
       </c>
@@ -931,7 +969,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>54</v>
       </c>
@@ -945,7 +983,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>46</v>
       </c>
@@ -959,7 +997,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>56</v>
       </c>
@@ -973,7 +1011,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>42</v>
       </c>
@@ -987,7 +1025,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>44</v>
       </c>
@@ -1001,7 +1039,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>45</v>
       </c>
@@ -1015,7 +1053,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>44</v>
       </c>
@@ -1029,7 +1067,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>42</v>
       </c>
@@ -1043,7 +1081,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>46</v>
       </c>
@@ -1057,7 +1095,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>48</v>
       </c>
@@ -1071,7 +1109,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>45</v>
       </c>
@@ -1085,7 +1123,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>87</v>
       </c>
@@ -1099,7 +1137,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>102</v>
       </c>
@@ -1113,7 +1151,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>101</v>
       </c>
@@ -1127,7 +1165,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>93</v>
       </c>
@@ -1141,7 +1179,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>101</v>
       </c>
@@ -1155,7 +1193,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>96</v>
       </c>
@@ -1169,7 +1207,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>94</v>
       </c>
@@ -1183,7 +1221,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>94</v>
       </c>
@@ -1197,7 +1235,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>91</v>
       </c>
@@ -1211,7 +1249,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>77</v>
       </c>
@@ -1225,7 +1263,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>90</v>
       </c>
@@ -1239,7 +1277,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>99</v>
       </c>
@@ -1253,7 +1291,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>84</v>
       </c>
@@ -1267,7 +1305,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>82</v>
       </c>
@@ -1281,7 +1319,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>83</v>
       </c>
@@ -1295,7 +1333,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>74</v>
       </c>
@@ -1309,7 +1347,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>63</v>
       </c>
@@ -1323,7 +1361,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>76</v>
       </c>
@@ -1337,7 +1375,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>81</v>
       </c>
@@ -1351,7 +1389,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>78</v>
       </c>
@@ -1365,7 +1403,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>79</v>
       </c>
@@ -1379,7 +1417,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>78</v>
       </c>
@@ -1393,7 +1431,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>79</v>
       </c>
@@ -1407,7 +1445,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>82</v>
       </c>
@@ -1421,7 +1459,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>82</v>
       </c>
@@ -1435,7 +1473,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>84</v>
       </c>
@@ -1449,7 +1487,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>86</v>
       </c>
@@ -1463,7 +1501,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>76</v>
       </c>
@@ -1477,7 +1515,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>74</v>
       </c>
@@ -1491,7 +1529,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>74</v>
       </c>
@@ -1505,7 +1543,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>66</v>
       </c>
@@ -1519,7 +1557,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>75</v>
       </c>
@@ -1533,7 +1571,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>71</v>
       </c>
@@ -1547,7 +1585,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>78</v>
       </c>
@@ -1561,7 +1599,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>73</v>
       </c>
@@ -1575,7 +1613,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>75</v>
       </c>
@@ -1589,7 +1627,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>69</v>
       </c>
@@ -1603,7 +1641,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>72</v>
       </c>
@@ -1617,7 +1655,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>72</v>
       </c>
@@ -1631,7 +1669,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>65</v>
       </c>
@@ -1645,7 +1683,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1659,7 +1697,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>64</v>
       </c>
@@ -1673,7 +1711,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>63</v>
       </c>
@@ -1687,7 +1725,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>70</v>
       </c>
@@ -1701,7 +1739,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>71</v>
       </c>
@@ -1715,7 +1753,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>67</v>
       </c>
@@ -1729,7 +1767,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>62</v>
       </c>
@@ -1743,7 +1781,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>68</v>
       </c>
@@ -1757,7 +1795,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>69</v>
       </c>
@@ -1771,7 +1809,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>66</v>
       </c>
@@ -1785,7 +1823,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>61</v>
       </c>
@@ -1799,7 +1837,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>61</v>
       </c>
@@ -1813,7 +1851,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>111</v>
       </c>
@@ -1827,7 +1865,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>106</v>
       </c>
@@ -1841,7 +1879,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>101</v>
       </c>
@@ -1855,7 +1893,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>126</v>
       </c>
@@ -1869,7 +1907,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>128</v>
       </c>
@@ -1883,7 +1921,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>129</v>
       </c>
@@ -1897,7 +1935,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>129</v>
       </c>
@@ -1911,7 +1949,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>111</v>
       </c>
@@ -1925,7 +1963,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>119</v>
       </c>
@@ -1939,7 +1977,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>111</v>
       </c>
@@ -1953,7 +1991,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>114</v>
       </c>
@@ -1967,7 +2005,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>121</v>
       </c>
@@ -1981,7 +2019,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>92</v>
       </c>
@@ -1995,7 +2033,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>85</v>
       </c>
@@ -2009,7 +2047,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>84</v>
       </c>
@@ -2023,7 +2061,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2037,7 +2075,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>90</v>
       </c>
@@ -2051,7 +2089,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>78</v>
       </c>
@@ -2065,7 +2103,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>89</v>
       </c>
@@ -2079,7 +2117,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>87</v>
       </c>
@@ -2093,7 +2131,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>107</v>
       </c>
@@ -2107,7 +2145,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>87</v>
       </c>
@@ -2121,7 +2159,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>84</v>
       </c>
@@ -2135,7 +2173,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>86</v>
       </c>
@@ -2149,7 +2187,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>120</v>
       </c>
@@ -2163,7 +2201,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>133</v>
       </c>
@@ -2177,7 +2215,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>131</v>
       </c>
@@ -2191,7 +2229,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>124</v>
       </c>
@@ -2205,7 +2243,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>119</v>
       </c>
@@ -2219,7 +2257,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>115</v>
       </c>
@@ -2233,7 +2271,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>125</v>
       </c>
@@ -2247,7 +2285,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>114</v>
       </c>
@@ -2261,7 +2299,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>123</v>
       </c>
@@ -2275,7 +2313,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>120</v>
       </c>
@@ -2289,7 +2327,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>113</v>
       </c>
@@ -2303,7 +2341,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>132</v>
       </c>
@@ -2317,7 +2355,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>99</v>
       </c>
@@ -2331,7 +2369,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>98</v>
       </c>
@@ -2345,7 +2383,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>90</v>
       </c>
@@ -2359,7 +2397,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>91</v>
       </c>
@@ -2373,7 +2411,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>86</v>
       </c>
@@ -2387,7 +2425,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>93</v>
       </c>
@@ -2401,7 +2439,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>88</v>
       </c>
@@ -2415,7 +2453,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>87</v>
       </c>
@@ -2429,7 +2467,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>86</v>
       </c>
@@ -2443,7 +2481,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>91</v>
       </c>
@@ -2457,7 +2495,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>92</v>
       </c>
@@ -2471,7 +2509,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>110</v>
       </c>
@@ -2485,7 +2523,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>110</v>
       </c>
@@ -2499,7 +2537,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>102</v>
       </c>
@@ -2513,7 +2551,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>100</v>
       </c>
@@ -2527,7 +2565,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>92</v>
       </c>
@@ -2541,7 +2579,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>114</v>
       </c>
@@ -2555,7 +2593,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>113</v>
       </c>
@@ -2569,7 +2607,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>106</v>
       </c>
@@ -2583,7 +2621,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>78</v>
       </c>
@@ -2597,7 +2635,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>80</v>
       </c>
@@ -2611,7 +2649,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>77</v>
       </c>
@@ -2625,7 +2663,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>82</v>
       </c>
@@ -2639,7 +2677,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>77</v>
       </c>
@@ -2653,7 +2691,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>78</v>
       </c>
@@ -2667,7 +2705,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>87</v>
       </c>
@@ -2681,7 +2719,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>88</v>
       </c>
@@ -2695,7 +2733,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>83</v>
       </c>
@@ -2709,7 +2747,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>76</v>
       </c>
@@ -2723,7 +2761,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>80</v>
       </c>
@@ -2737,7 +2775,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>73</v>
       </c>
@@ -2751,7 +2789,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>75</v>
       </c>
@@ -2765,7 +2803,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>74</v>
       </c>
@@ -2779,7 +2817,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>69</v>
       </c>
@@ -2793,7 +2831,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>73</v>
       </c>
@@ -2807,7 +2845,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>89</v>
       </c>
@@ -2821,7 +2859,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>91</v>
       </c>
@@ -2835,7 +2873,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>86</v>
       </c>
@@ -2849,7 +2887,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>84</v>
       </c>
@@ -2863,7 +2901,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>102</v>
       </c>
@@ -2877,7 +2915,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>93</v>
       </c>
@@ -2891,7 +2929,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>77</v>
       </c>
@@ -2905,7 +2943,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>99</v>
       </c>
@@ -2919,7 +2957,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>97</v>
       </c>
@@ -2933,7 +2971,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>95</v>
       </c>
@@ -2947,7 +2985,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>88</v>
       </c>
@@ -2961,7 +2999,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>80</v>
       </c>
@@ -2975,7 +3013,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>78</v>
       </c>
@@ -2989,7 +3027,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>75</v>
       </c>
@@ -3003,7 +3041,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>68</v>
       </c>
@@ -3017,7 +3055,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>68</v>
       </c>
@@ -3031,7 +3069,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>66</v>
       </c>
@@ -3045,7 +3083,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>65</v>
       </c>
@@ -3059,7 +3097,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>73</v>
       </c>
@@ -3073,7 +3111,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>77</v>
       </c>
@@ -3087,7 +3125,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>70</v>
       </c>
@@ -3101,7 +3139,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>66</v>
       </c>
@@ -3115,7 +3153,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>75</v>
       </c>
@@ -3129,7 +3167,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>74</v>
       </c>
@@ -3143,7 +3181,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>129</v>
       </c>
@@ -3157,7 +3195,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>128</v>
       </c>
@@ -3171,7 +3209,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>115</v>
       </c>
@@ -3185,7 +3223,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>117</v>
       </c>
@@ -3199,7 +3237,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>142</v>
       </c>
@@ -3213,7 +3251,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>138</v>
       </c>
@@ -3227,7 +3265,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>137</v>
       </c>
@@ -3241,7 +3279,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>130</v>
       </c>
@@ -3255,7 +3293,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>124</v>
       </c>
@@ -3269,7 +3307,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>130</v>
       </c>
@@ -3283,7 +3321,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>129</v>
       </c>
@@ -3297,7 +3335,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>121</v>
       </c>
@@ -3311,7 +3349,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>115</v>
       </c>
@@ -3325,7 +3363,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>117</v>
       </c>
@@ -3339,7 +3377,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>123</v>
       </c>
@@ -3353,7 +3391,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>118</v>
       </c>
@@ -3367,7 +3405,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>124</v>
       </c>
@@ -3381,7 +3419,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>128</v>
       </c>
@@ -3395,7 +3433,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>122</v>
       </c>
@@ -3409,7 +3447,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>125</v>
       </c>
@@ -3423,7 +3461,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>118</v>
       </c>
@@ -3437,7 +3475,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>125</v>
       </c>
@@ -3448,7 +3486,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>124</v>
       </c>
@@ -3459,7 +3497,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>121</v>
       </c>
@@ -3470,7 +3508,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>149</v>
       </c>
@@ -3481,7 +3519,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>147</v>
       </c>
@@ -3492,7 +3530,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>151</v>
       </c>
@@ -3503,7 +3541,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>142</v>
       </c>
@@ -3514,7 +3552,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>132</v>
       </c>
@@ -3525,7 +3563,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>132</v>
       </c>
@@ -3536,7 +3574,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>141</v>
       </c>
@@ -3544,7 +3582,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>140</v>
       </c>
@@ -3552,7 +3590,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>133</v>
       </c>
@@ -3560,7 +3598,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>139</v>
       </c>
@@ -3568,7 +3606,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>148</v>
       </c>
@@ -3576,7 +3614,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>138</v>
       </c>
@@ -3584,7 +3622,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>127</v>
       </c>
@@ -3592,7 +3630,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>135</v>
       </c>
@@ -3600,7 +3638,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>133</v>
       </c>
@@ -3608,7 +3646,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>141</v>
       </c>
@@ -3616,7 +3654,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>142</v>
       </c>
@@ -3624,7 +3662,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>129</v>
       </c>
@@ -3632,7 +3670,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>126</v>
       </c>
@@ -3640,7 +3678,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>130</v>
       </c>
@@ -3648,7 +3686,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>134</v>
       </c>
@@ -3656,7 +3694,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>136</v>
       </c>
@@ -3664,7 +3702,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>138</v>
       </c>
@@ -3672,7 +3710,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>117</v>
       </c>
@@ -3680,7 +3718,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>118</v>
       </c>
@@ -3688,7 +3726,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>104</v>
       </c>
@@ -3696,7 +3734,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>148</v>
       </c>
@@ -3704,7 +3742,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>151</v>
       </c>
@@ -3712,7 +3750,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>144</v>
       </c>
@@ -3720,7 +3758,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>157</v>
       </c>
@@ -3728,7 +3766,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>147</v>
       </c>
@@ -3736,7 +3774,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>152</v>
       </c>
@@ -3744,7 +3782,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>154</v>
       </c>
@@ -3752,7 +3790,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>142</v>
       </c>
@@ -3760,7 +3798,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>129</v>
       </c>
@@ -3768,7 +3806,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>135</v>
       </c>
@@ -3776,7 +3814,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>130</v>
       </c>
@@ -3784,7 +3822,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>130</v>
       </c>
@@ -3792,7 +3830,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>120</v>
       </c>
@@ -3800,7 +3838,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>105</v>
       </c>
@@ -3808,7 +3846,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>111</v>
       </c>
@@ -3816,7 +3854,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>114</v>
       </c>
@@ -3824,7 +3862,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>116</v>
       </c>
@@ -3832,7 +3870,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>131</v>
       </c>
@@ -3840,7 +3878,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>105</v>
       </c>
@@ -3848,7 +3886,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>109</v>
       </c>
@@ -3856,7 +3894,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>101</v>
       </c>
@@ -3864,7 +3902,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>94</v>
       </c>
@@ -3872,7 +3910,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>92</v>
       </c>
@@ -3880,7 +3918,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>92</v>
       </c>
@@ -3888,7 +3926,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>94</v>
       </c>
@@ -3896,7 +3934,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>96</v>
       </c>
@@ -3904,7 +3942,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>95</v>
       </c>
@@ -3912,7 +3950,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>93</v>
       </c>
@@ -3920,7 +3958,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>83</v>
       </c>
@@ -3928,7 +3966,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>84</v>
       </c>
@@ -3936,7 +3974,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>88</v>
       </c>
@@ -3944,7 +3982,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>90</v>
       </c>
@@ -3952,7 +3990,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>88</v>
       </c>
@@ -3960,7 +3998,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>85</v>
       </c>
@@ -3968,7 +4006,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>76</v>
       </c>
@@ -3976,7 +4014,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>89</v>
       </c>
@@ -3984,7 +4022,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>76</v>
       </c>
@@ -3992,7 +4030,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>81</v>
       </c>
@@ -4000,7 +4038,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>83</v>
       </c>
@@ -4008,7 +4046,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>79</v>
       </c>
@@ -4016,7 +4054,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>72</v>
       </c>
@@ -4024,7 +4062,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>76</v>
       </c>
@@ -4032,7 +4070,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>81</v>
       </c>
@@ -4040,7 +4078,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>85</v>
       </c>
@@ -4048,7 +4086,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>80</v>
       </c>
@@ -4056,7 +4094,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>140</v>
       </c>
@@ -4064,7 +4102,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>122</v>
       </c>
@@ -4072,7 +4110,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>141</v>
       </c>
@@ -4080,7 +4118,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>129</v>
       </c>
@@ -4088,7 +4126,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>124</v>
       </c>
@@ -4096,7 +4134,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>128</v>
       </c>
@@ -4104,7 +4142,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>121</v>
       </c>
@@ -4112,7 +4150,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>120</v>
       </c>
@@ -4120,7 +4158,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>114</v>
       </c>
@@ -4128,7 +4166,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>117</v>
       </c>
@@ -4136,7 +4174,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>125</v>
       </c>
@@ -4144,7 +4182,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>104</v>
       </c>
@@ -4152,7 +4190,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>115</v>
       </c>
@@ -4160,7 +4198,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>115</v>
       </c>
@@ -4168,7 +4206,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>115</v>
       </c>
@@ -4176,7 +4214,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>110</v>
       </c>
@@ -4184,7 +4222,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>113</v>
       </c>
@@ -4192,7 +4230,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>113</v>
       </c>
@@ -4200,7 +4238,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>102</v>
       </c>
@@ -4208,7 +4246,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>103</v>
       </c>
@@ -4216,7 +4254,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>102</v>
       </c>
@@ -4224,7 +4262,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>126</v>
       </c>
@@ -4232,7 +4270,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>115</v>
       </c>
@@ -4240,7 +4278,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>112</v>
       </c>
@@ -4248,7 +4286,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>129</v>
       </c>
@@ -4256,7 +4294,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>126</v>
       </c>
@@ -4264,7 +4302,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>135</v>
       </c>
@@ -4272,7 +4310,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>133</v>
       </c>
@@ -4280,7 +4318,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>136</v>
       </c>
@@ -4288,7 +4326,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>129</v>
       </c>
@@ -4296,7 +4334,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>130</v>
       </c>
@@ -4304,7 +4342,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>112</v>
       </c>
@@ -4312,7 +4350,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>119</v>
       </c>
@@ -4320,7 +4358,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>125</v>
       </c>
@@ -4328,7 +4366,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>114</v>
       </c>
@@ -4336,7 +4374,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>113</v>
       </c>
@@ -4344,7 +4382,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>127</v>
       </c>
@@ -4352,7 +4390,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>105</v>
       </c>
@@ -4360,7 +4398,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>107</v>
       </c>
@@ -4368,7 +4406,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>113</v>
       </c>
@@ -4376,7 +4414,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>112</v>
       </c>
@@ -4384,7 +4422,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>110</v>
       </c>
@@ -4392,7 +4430,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>110</v>
       </c>
@@ -4400,7 +4438,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>108</v>
       </c>
@@ -4408,7 +4446,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>106</v>
       </c>
@@ -4416,7 +4454,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>101</v>
       </c>
@@ -4424,7 +4462,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>112</v>
       </c>
@@ -4432,7 +4470,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>114</v>
       </c>
@@ -4440,7 +4478,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>68</v>
       </c>
@@ -4448,7 +4486,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>66</v>
       </c>
@@ -4456,7 +4494,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>67</v>
       </c>
@@ -4464,7 +4502,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>63</v>
       </c>
@@ -4472,7 +4510,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>65</v>
       </c>
@@ -4480,7 +4518,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>70</v>
       </c>
@@ -4488,7 +4526,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>66</v>
       </c>
@@ -4496,7 +4534,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>61</v>
       </c>
@@ -4504,7 +4542,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>60</v>
       </c>
@@ -4512,7 +4550,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>68</v>
       </c>
@@ -4520,7 +4558,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>60</v>
       </c>
@@ -4528,7 +4566,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>53</v>
       </c>
@@ -4536,7 +4574,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>64</v>
       </c>
@@ -4544,7 +4582,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>66</v>
       </c>
@@ -4552,7 +4590,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>59</v>
       </c>
@@ -4560,7 +4598,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>65</v>
       </c>
@@ -4568,7 +4606,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>55</v>
       </c>
@@ -4576,7 +4614,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>69</v>
       </c>
@@ -4584,7 +4622,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>67</v>
       </c>
@@ -4592,7 +4630,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>69</v>
       </c>
@@ -4600,7 +4638,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>63</v>
       </c>
@@ -4608,7 +4646,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>65</v>
       </c>
@@ -4616,7 +4654,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>70</v>
       </c>
@@ -4624,7 +4662,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>65</v>
       </c>
@@ -4632,7 +4670,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>104</v>
       </c>
@@ -4640,7 +4678,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>121</v>
       </c>
@@ -4648,7 +4686,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>108</v>
       </c>
@@ -4656,7 +4694,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>105</v>
       </c>
@@ -4664,7 +4702,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>106</v>
       </c>
@@ -4672,7 +4710,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>115</v>
       </c>
@@ -4680,7 +4718,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>108</v>
       </c>
@@ -4688,7 +4726,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>104</v>
       </c>
@@ -4696,7 +4734,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>111</v>
       </c>
@@ -4704,7 +4742,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>99</v>
       </c>
@@ -4712,7 +4750,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>100</v>
       </c>
@@ -4720,7 +4758,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>108</v>
       </c>
@@ -4728,7 +4766,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>99</v>
       </c>
@@ -4736,7 +4774,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>101</v>
       </c>
@@ -4744,7 +4782,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>99</v>
       </c>
@@ -4752,7 +4790,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>91</v>
       </c>
@@ -4760,7 +4798,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>90</v>
       </c>
@@ -4768,7 +4806,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>90</v>
       </c>
@@ -4776,7 +4814,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>94</v>
       </c>
@@ -4784,7 +4822,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>91</v>
       </c>
@@ -4792,7 +4830,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>95</v>
       </c>
@@ -4800,7 +4838,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>95</v>
       </c>
@@ -4808,7 +4846,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>89</v>
       </c>
@@ -4816,7 +4854,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>90</v>
       </c>
@@ -4824,7 +4862,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>124</v>
       </c>
@@ -4832,7 +4870,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>110</v>
       </c>
@@ -4840,7 +4878,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>110</v>
       </c>
@@ -4848,7 +4886,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>103</v>
       </c>
@@ -4856,7 +4894,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>110</v>
       </c>
@@ -4864,7 +4902,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>107</v>
       </c>
@@ -4872,7 +4910,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>117</v>
       </c>
@@ -4880,7 +4918,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>110</v>
       </c>
@@ -4888,7 +4926,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>112</v>
       </c>
@@ -4896,7 +4934,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>117</v>
       </c>
@@ -4904,7 +4942,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>108</v>
       </c>
@@ -4912,7 +4950,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>109</v>
       </c>
@@ -4920,422 +4958,422 @@
         <v>91</v>
       </c>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>101</v>
       </c>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>110</v>
       </c>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>92</v>
       </c>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>95</v>
       </c>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>91</v>
       </c>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>95</v>
       </c>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>92</v>
       </c>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>95</v>
       </c>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>108</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>110</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>102</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>100</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>118</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>112</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>117</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>107</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>110</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>109</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>102</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>105</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>99</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>104</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>91</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>104</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>91</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>92</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>94</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>94</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>105</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>102</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>91</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>98</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>93</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>96</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>101</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>94</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>83</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>80</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>82</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415">
         <v>73</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416">
         <v>76</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>71</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>73</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>71</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>75</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>83</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>92</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>86</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>92</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>88</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>79</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427">
         <v>80</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>77</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A429">
         <v>77</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A430">
         <v>77</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A431">
         <v>75</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432">
         <v>81</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433">
         <v>78</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A434">
         <v>79</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A435">
         <v>80</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A436">
         <v>95</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A437">
         <v>79</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A438">
         <v>87</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A439">
         <v>80</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A440">
         <v>81</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A441">
         <v>84</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A442">
         <v>73</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A443">
         <v>84</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A444">
         <v>84</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445">
         <v>92</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A446">
         <v>84</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447">
         <v>89</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A448">
         <v>81</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A449">
         <v>73</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A450">
         <v>62</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A451">
         <v>79</v>
       </c>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A452">
         <v>76</v>
       </c>
     </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A453">
         <v>76</v>
       </c>
     </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A454">
         <v>77</v>
       </c>
     </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A455">
         <v>71</v>
       </c>
     </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A456">
         <v>81</v>
       </c>
     </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A457">
         <v>79</v>
       </c>
     </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A458">
         <v>78</v>
       </c>
     </row>
-    <row r="459" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A459">
         <v>80</v>
       </c>

</xml_diff>